<commit_message>
Stage 2 check jawaban
</commit_message>
<xml_diff>
--- a/Pola Jawaban.xlsx
+++ b/Pola Jawaban.xlsx
@@ -1056,14 +1056,14 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1581,7 +1581,9 @@
       <c r="U10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="V10" s="4"/>
+      <c r="V10" s="4">
+        <v>102</v>
+      </c>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="1"/>

</xml_diff>

<commit_message>
Hint function stage 2
</commit_message>
<xml_diff>
--- a/Pola Jawaban.xlsx
+++ b/Pola Jawaban.xlsx
@@ -1056,7 +1056,7 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,10 +1515,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>

</xml_diff>